<commit_message>
modificacion de clases de excel etc
</commit_message>
<xml_diff>
--- a/plantilla-alta_beneficiarios_pension.xlsx
+++ b/plantilla-alta_beneficiarios_pension.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\generar_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17EC2CD-FAE1-4260-8AEC-9A283DC7AD7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3613EDE-CFBE-472A-A091-39476164CCE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="plantilla" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
@@ -35,7 +35,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -68,6 +68,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -89,16 +95,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:P7"/>
+  <dimension ref="A2:P8"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,18 +532,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:16" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -550,14 +557,17 @@
       <c r="P4" s="1"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C8" s="5"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>